<commit_message>
filtrar de alimentos y peces filas de  estado reportado, mover nombre de empresa en tabla resumen, agregar fila de peces analizados
</commit_message>
<xml_diff>
--- a/src/assets/Test-Reporte_Elanco/Alimento.xlsx
+++ b/src/assets/Test-Reporte_Elanco/Alimento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catta\Desktop\Test-Reporte_Elanco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catta\Documents\COMPSCI\repos\elanco-infome-imvixa\src\assets\Test-Reporte_Elanco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340B8BF8-4438-43E8-B5EA-901860BC0014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA90B13-A899-45DA-BE61-1C6BDF81AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alimento" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="115">
   <si>
     <t>Estado</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>2020-002</t>
+  </si>
+  <si>
+    <t>InReportado</t>
   </si>
 </sst>
 </file>
@@ -375,8 +378,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -500,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -532,13 +535,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -571,6 +574,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,13 +877,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1651,6 +1684,166 @@
         <v>6.4153541772720831E-3</v>
       </c>
       <c r="Z10" s="13">
+        <v>0.96484375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="6">
+        <v>43850</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" s="8">
+        <v>2740</v>
+      </c>
+      <c r="M11" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="N11" s="7">
+        <v>320</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>43857</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="8">
+        <v>309.60000000000002</v>
+      </c>
+      <c r="T11" s="8">
+        <v>307.60000000000002</v>
+      </c>
+      <c r="U11" s="8">
+        <v>306.7</v>
+      </c>
+      <c r="V11" s="8">
+        <v>311.10000000000002</v>
+      </c>
+      <c r="W11" s="10">
+        <v>308.75</v>
+      </c>
+      <c r="X11" s="11">
+        <v>1.9807406022327556</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>6.4153541772720831E-3</v>
+      </c>
+      <c r="Z11" s="13">
+        <v>0.96484375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="25">
+        <v>43850</v>
+      </c>
+      <c r="C12" s="26">
+        <v>2020</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="L12" s="27">
+        <v>2740</v>
+      </c>
+      <c r="M12" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="N12" s="26">
+        <v>320</v>
+      </c>
+      <c r="O12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="P12" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="25">
+        <v>43857</v>
+      </c>
+      <c r="R12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" s="27">
+        <v>309.60000000000002</v>
+      </c>
+      <c r="T12" s="27">
+        <v>307.60000000000002</v>
+      </c>
+      <c r="U12" s="27">
+        <v>306.7</v>
+      </c>
+      <c r="V12" s="27">
+        <v>311.10000000000002</v>
+      </c>
+      <c r="W12" s="29">
+        <v>308.75</v>
+      </c>
+      <c r="X12" s="30">
+        <v>1.9807406022327556</v>
+      </c>
+      <c r="Y12" s="12">
+        <v>6.4153541772720831E-3</v>
+      </c>
+      <c r="Z12" s="13">
         <v>0.96484375</v>
       </c>
     </row>
@@ -1663,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13FA2C19-C54A-498A-8DA2-7DB76BB6E036}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
hacer funcionar con planillas nuevas
</commit_message>
<xml_diff>
--- a/src/assets/Test-Reporte_Elanco/Alimento.xlsx
+++ b/src/assets/Test-Reporte_Elanco/Alimento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catta\Documents\COMPSCI\repos\elanco-infome-imvixa\src\assets\Test-Reporte_Elanco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA90B13-A899-45DA-BE61-1C6BDF81AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDDC580-C862-4425-B104-024086DEC924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alimento" sheetId="1" r:id="rId1"/>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13FA2C19-C54A-498A-8DA2-7DB76BB6E036}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>